<commit_message>
Ver vehículos, modelos, marcas, reportar gastos
</commit_message>
<xml_diff>
--- a/Documentación/Rubricas.xlsx
+++ b/Documentación/Rubricas.xlsx
@@ -856,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1117,7 +1117,9 @@
       <c r="C19" s="4">
         <v>1</v>
       </c>
-      <c r="D19" s="8"/>
+      <c r="D19" s="8">
+        <v>1</v>
+      </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
     </row>
@@ -1129,7 +1131,9 @@
       <c r="C20" s="4">
         <v>1</v>
       </c>
-      <c r="D20" s="8"/>
+      <c r="D20" s="8">
+        <v>1</v>
+      </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
     </row>
@@ -1285,7 +1289,7 @@
       </c>
       <c r="D32" s="11">
         <f>SUM(D3:D31)</f>
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E32" s="19"/>
       <c r="F32" s="20"/>

</xml_diff>